<commit_message>
add [035]、[036] files and data
</commit_message>
<xml_diff>
--- a/DataGraph[027-041]/data/accounts.xlsx
+++ b/DataGraph[027-041]/data/accounts.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\PythonBooks\1 开发资源库\编程1小时\2020年第6期\按年统计日常消费数据【Pandas专题】\python20200115code01\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\05_job src\programming_practice_project\DataGraph[027-041]\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83947068-A2D8-4E3C-821A-5D6985ABCA9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16125" windowHeight="8145"/>
+    <workbookView xWindow="-2508" yWindow="4788" windowWidth="23040" windowHeight="7944" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -626,7 +627,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -825,16 +826,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="表3" displayName="表3" ref="A1:D147" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
-  <autoFilter ref="A1:D147"/>
-  <sortState ref="A2:D26">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="表3" displayName="表3" ref="A1:D147" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="A1:D147" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D26">
     <sortCondition ref="A1"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" name="日期" dataDxfId="3"/>
-    <tableColumn id="2" name="名称" dataDxfId="2"/>
-    <tableColumn id="3" name="支出类别" dataDxfId="1"/>
-    <tableColumn id="4" name="金额" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="日期" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="名称" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="支出类别" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="金额" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1102,21 +1103,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A131" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H137" sqref="H137"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.5" customWidth="1"/>
-    <col min="2" max="2" width="20.375" customWidth="1"/>
-    <col min="3" max="3" width="12.625" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1130,7 +1132,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>43618</v>
       </c>
@@ -1144,7 +1146,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>43619</v>
       </c>
@@ -1158,7 +1160,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>43620</v>
       </c>
@@ -1172,7 +1174,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>43639</v>
       </c>
@@ -1186,7 +1188,7 @@
         <v>205.3</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>43670</v>
       </c>
@@ -1200,7 +1202,7 @@
         <v>118.7</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>43671</v>
       </c>
@@ -1214,7 +1216,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>43672</v>
       </c>
@@ -1228,7 +1230,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>43673</v>
       </c>
@@ -1242,7 +1244,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>43679</v>
       </c>
@@ -1256,7 +1258,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>43706</v>
       </c>
@@ -1270,7 +1272,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>43707</v>
       </c>
@@ -1284,7 +1286,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>43708</v>
       </c>
@@ -1298,7 +1300,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>43709</v>
       </c>
@@ -1312,7 +1314,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>43710</v>
       </c>
@@ -1326,7 +1328,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>43711</v>
       </c>
@@ -1340,7 +1342,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>43712</v>
       </c>
@@ -1354,7 +1356,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>43713</v>
       </c>
@@ -1368,7 +1370,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>43728</v>
       </c>
@@ -1382,7 +1384,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>43739</v>
       </c>
@@ -1396,7 +1398,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>43770</v>
       </c>
@@ -1410,7 +1412,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>43780</v>
       </c>
@@ -1424,7 +1426,7 @@
         <v>778.5</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>43800</v>
       </c>
@@ -1438,7 +1440,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>43801</v>
       </c>
@@ -1452,7 +1454,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>43802</v>
       </c>
@@ -1466,7 +1468,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>43802</v>
       </c>
@@ -1480,7 +1482,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>43803</v>
       </c>
@@ -1494,7 +1496,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>43804</v>
       </c>
@@ -1508,7 +1510,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>43805</v>
       </c>
@@ -1522,7 +1524,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>43806</v>
       </c>
@@ -1536,7 +1538,7 @@
         <v>79.8</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>43806</v>
       </c>
@@ -1550,7 +1552,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>43807</v>
       </c>
@@ -1564,7 +1566,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>43808</v>
       </c>
@@ -1578,7 +1580,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>43809</v>
       </c>
@@ -1592,7 +1594,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>43809</v>
       </c>
@@ -1606,7 +1608,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>43810</v>
       </c>
@@ -1620,7 +1622,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>43811</v>
       </c>
@@ -1634,7 +1636,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>43822</v>
       </c>
@@ -1648,7 +1650,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>43823</v>
       </c>
@@ -1662,7 +1664,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>43823</v>
       </c>
@@ -1676,7 +1678,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>43824</v>
       </c>
@@ -1690,7 +1692,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>43825</v>
       </c>
@@ -1704,7 +1706,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>43826</v>
       </c>
@@ -1718,7 +1720,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>43827</v>
       </c>
@@ -1732,7 +1734,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>43828</v>
       </c>
@@ -1746,7 +1748,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>43829</v>
       </c>
@@ -1760,7 +1762,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>43830</v>
       </c>
@@ -1774,7 +1776,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>43182</v>
       </c>
@@ -1788,7 +1790,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>43305</v>
       </c>
@@ -1802,7 +1804,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>43306</v>
       </c>
@@ -1816,7 +1818,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>43307</v>
       </c>
@@ -1830,7 +1832,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>43308</v>
       </c>
@@ -1844,7 +1846,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>43314</v>
       </c>
@@ -1858,7 +1860,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>43341</v>
       </c>
@@ -1872,7 +1874,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>43342</v>
       </c>
@@ -1886,7 +1888,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>43343</v>
       </c>
@@ -1900,7 +1902,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>43344</v>
       </c>
@@ -1914,7 +1916,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>43345</v>
       </c>
@@ -1928,7 +1930,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>43346</v>
       </c>
@@ -1942,7 +1944,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>43347</v>
       </c>
@@ -1956,7 +1958,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>43348</v>
       </c>
@@ -1970,7 +1972,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>43363</v>
       </c>
@@ -1984,7 +1986,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>43374</v>
       </c>
@@ -1998,7 +2000,7 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>43388</v>
       </c>
@@ -2012,7 +2014,7 @@
         <v>3200</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>43415</v>
       </c>
@@ -2026,7 +2028,7 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>43435</v>
       </c>
@@ -2040,7 +2042,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:4" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>43436</v>
       </c>
@@ -2054,488 +2056,488 @@
         <v>200</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="4"/>
       <c r="B68" s="5"/>
       <c r="C68" s="5"/>
       <c r="D68" s="5"/>
     </row>
-    <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="4"/>
       <c r="B69" s="5"/>
       <c r="C69" s="5"/>
       <c r="D69" s="5"/>
     </row>
-    <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="4"/>
       <c r="B70" s="5"/>
       <c r="C70" s="5"/>
       <c r="D70" s="5"/>
     </row>
-    <row r="71" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="4"/>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
       <c r="D71" s="5"/>
     </row>
-    <row r="72" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="4"/>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
       <c r="D72" s="5"/>
     </row>
-    <row r="73" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="4"/>
       <c r="B73" s="5"/>
       <c r="C73" s="5"/>
       <c r="D73" s="5"/>
     </row>
-    <row r="74" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="4"/>
       <c r="B74" s="5"/>
       <c r="C74" s="5"/>
       <c r="D74" s="5"/>
     </row>
-    <row r="75" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="4"/>
       <c r="B75" s="5"/>
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
     </row>
-    <row r="76" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="4"/>
       <c r="B76" s="5"/>
       <c r="C76" s="5"/>
       <c r="D76" s="5"/>
     </row>
-    <row r="77" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="4"/>
       <c r="B77" s="5"/>
       <c r="C77" s="5"/>
       <c r="D77" s="5"/>
     </row>
-    <row r="78" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="4"/>
       <c r="B78" s="5"/>
       <c r="C78" s="5"/>
       <c r="D78" s="5"/>
     </row>
-    <row r="79" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="4"/>
       <c r="B79" s="5"/>
       <c r="C79" s="5"/>
       <c r="D79" s="5"/>
     </row>
-    <row r="80" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="4"/>
       <c r="B80" s="5"/>
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
     </row>
-    <row r="81" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="4"/>
       <c r="B81" s="5"/>
       <c r="C81" s="5"/>
       <c r="D81" s="5"/>
     </row>
-    <row r="82" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="4"/>
       <c r="B82" s="5"/>
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
     </row>
-    <row r="83" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="4"/>
       <c r="B83" s="5"/>
       <c r="C83" s="5"/>
       <c r="D83" s="5"/>
     </row>
-    <row r="84" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A84" s="4"/>
       <c r="B84" s="5"/>
       <c r="C84" s="5"/>
       <c r="D84" s="5"/>
     </row>
-    <row r="85" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="4"/>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
       <c r="D85" s="5"/>
     </row>
-    <row r="86" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="4"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
       <c r="D86" s="5"/>
     </row>
-    <row r="87" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="4"/>
       <c r="B87" s="5"/>
       <c r="C87" s="5"/>
       <c r="D87" s="5"/>
     </row>
-    <row r="88" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="4"/>
       <c r="B88" s="5"/>
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
     </row>
-    <row r="89" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="4"/>
       <c r="B89" s="5"/>
       <c r="C89" s="5"/>
       <c r="D89" s="5"/>
     </row>
-    <row r="90" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="4"/>
       <c r="B90" s="5"/>
       <c r="C90" s="5"/>
       <c r="D90" s="5"/>
     </row>
-    <row r="91" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="4"/>
       <c r="B91" s="5"/>
       <c r="C91" s="5"/>
       <c r="D91" s="5"/>
     </row>
-    <row r="92" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="4"/>
       <c r="B92" s="5"/>
       <c r="C92" s="5"/>
       <c r="D92" s="5"/>
     </row>
-    <row r="93" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="4"/>
       <c r="B93" s="5"/>
       <c r="C93" s="5"/>
       <c r="D93" s="5"/>
     </row>
-    <row r="94" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="4"/>
       <c r="B94" s="5"/>
       <c r="C94" s="5"/>
       <c r="D94" s="5"/>
     </row>
-    <row r="95" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="4"/>
       <c r="B95" s="5"/>
       <c r="C95" s="5"/>
       <c r="D95" s="5"/>
     </row>
-    <row r="96" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="4"/>
       <c r="B96" s="5"/>
       <c r="C96" s="5"/>
       <c r="D96" s="5"/>
     </row>
-    <row r="97" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" s="4"/>
       <c r="B97" s="5"/>
       <c r="C97" s="5"/>
       <c r="D97" s="5"/>
     </row>
-    <row r="98" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" s="4"/>
       <c r="B98" s="5"/>
       <c r="C98" s="5"/>
       <c r="D98" s="5"/>
     </row>
-    <row r="99" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" s="4"/>
       <c r="B99" s="5"/>
       <c r="C99" s="5"/>
       <c r="D99" s="5"/>
     </row>
-    <row r="100" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" s="4"/>
       <c r="B100" s="5"/>
       <c r="C100" s="5"/>
       <c r="D100" s="5"/>
     </row>
-    <row r="101" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" s="4"/>
       <c r="B101" s="5"/>
       <c r="C101" s="5"/>
       <c r="D101" s="5"/>
     </row>
-    <row r="102" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" s="4"/>
       <c r="B102" s="5"/>
       <c r="C102" s="5"/>
       <c r="D102" s="5"/>
     </row>
-    <row r="103" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" s="4"/>
       <c r="B103" s="5"/>
       <c r="C103" s="5"/>
       <c r="D103" s="5"/>
     </row>
-    <row r="104" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" s="4"/>
       <c r="B104" s="5"/>
       <c r="C104" s="5"/>
       <c r="D104" s="5"/>
     </row>
-    <row r="105" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" s="4"/>
       <c r="B105" s="5"/>
       <c r="C105" s="5"/>
       <c r="D105" s="5"/>
     </row>
-    <row r="106" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" s="4"/>
       <c r="B106" s="5"/>
       <c r="C106" s="5"/>
       <c r="D106" s="5"/>
     </row>
-    <row r="107" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" s="4"/>
       <c r="B107" s="5"/>
       <c r="C107" s="5"/>
       <c r="D107" s="5"/>
     </row>
-    <row r="108" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" s="4"/>
       <c r="B108" s="5"/>
       <c r="C108" s="5"/>
       <c r="D108" s="5"/>
     </row>
-    <row r="109" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" s="4"/>
       <c r="B109" s="5"/>
       <c r="C109" s="5"/>
       <c r="D109" s="5"/>
     </row>
-    <row r="110" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" s="4"/>
       <c r="B110" s="5"/>
       <c r="C110" s="5"/>
       <c r="D110" s="5"/>
     </row>
-    <row r="111" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" s="4"/>
       <c r="B111" s="5"/>
       <c r="C111" s="5"/>
       <c r="D111" s="5"/>
     </row>
-    <row r="112" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" s="4"/>
       <c r="B112" s="5"/>
       <c r="C112" s="5"/>
       <c r="D112" s="5"/>
     </row>
-    <row r="113" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A113" s="4"/>
       <c r="B113" s="5"/>
       <c r="C113" s="5"/>
       <c r="D113" s="5"/>
     </row>
-    <row r="114" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A114" s="4"/>
       <c r="B114" s="5"/>
       <c r="C114" s="5"/>
       <c r="D114" s="5"/>
     </row>
-    <row r="115" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" s="4"/>
       <c r="B115" s="5"/>
       <c r="C115" s="5"/>
       <c r="D115" s="5"/>
     </row>
-    <row r="116" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A116" s="4"/>
       <c r="B116" s="5"/>
       <c r="C116" s="5"/>
       <c r="D116" s="5"/>
     </row>
-    <row r="117" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A117" s="4"/>
       <c r="B117" s="5"/>
       <c r="C117" s="5"/>
       <c r="D117" s="5"/>
     </row>
-    <row r="118" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A118" s="4"/>
       <c r="B118" s="5"/>
       <c r="C118" s="5"/>
       <c r="D118" s="5"/>
     </row>
-    <row r="119" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A119" s="4"/>
       <c r="B119" s="5"/>
       <c r="C119" s="5"/>
       <c r="D119" s="5"/>
     </row>
-    <row r="120" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A120" s="4"/>
       <c r="B120" s="5"/>
       <c r="C120" s="5"/>
       <c r="D120" s="5"/>
     </row>
-    <row r="121" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A121" s="4"/>
       <c r="B121" s="5"/>
       <c r="C121" s="5"/>
       <c r="D121" s="5"/>
     </row>
-    <row r="122" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A122" s="4"/>
       <c r="B122" s="5"/>
       <c r="C122" s="5"/>
       <c r="D122" s="5"/>
     </row>
-    <row r="123" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A123" s="4"/>
       <c r="B123" s="5"/>
       <c r="C123" s="5"/>
       <c r="D123" s="5"/>
     </row>
-    <row r="124" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A124" s="4"/>
       <c r="B124" s="5"/>
       <c r="C124" s="5"/>
       <c r="D124" s="5"/>
     </row>
-    <row r="125" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A125" s="4"/>
       <c r="B125" s="5"/>
       <c r="C125" s="5"/>
       <c r="D125" s="5"/>
     </row>
-    <row r="126" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A126" s="4"/>
       <c r="B126" s="5"/>
       <c r="C126" s="5"/>
       <c r="D126" s="5"/>
     </row>
-    <row r="127" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A127" s="4"/>
       <c r="B127" s="5"/>
       <c r="C127" s="5"/>
       <c r="D127" s="5"/>
     </row>
-    <row r="128" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A128" s="4"/>
       <c r="B128" s="5"/>
       <c r="C128" s="5"/>
       <c r="D128" s="5"/>
     </row>
-    <row r="129" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A129" s="4"/>
       <c r="B129" s="5"/>
       <c r="C129" s="5"/>
       <c r="D129" s="5"/>
     </row>
-    <row r="130" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" s="4"/>
       <c r="B130" s="5"/>
       <c r="C130" s="5"/>
       <c r="D130" s="5"/>
     </row>
-    <row r="131" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A131" s="4"/>
       <c r="B131" s="5"/>
       <c r="C131" s="5"/>
       <c r="D131" s="5"/>
     </row>
-    <row r="132" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A132" s="4"/>
       <c r="B132" s="5"/>
       <c r="C132" s="5"/>
       <c r="D132" s="5"/>
     </row>
-    <row r="133" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A133" s="4"/>
       <c r="B133" s="5"/>
       <c r="C133" s="5"/>
       <c r="D133" s="5"/>
     </row>
-    <row r="134" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A134" s="4"/>
       <c r="B134" s="5"/>
       <c r="C134" s="5"/>
       <c r="D134" s="5"/>
     </row>
-    <row r="135" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A135" s="4"/>
       <c r="B135" s="5"/>
       <c r="C135" s="5"/>
       <c r="D135" s="5"/>
     </row>
-    <row r="136" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A136" s="4"/>
       <c r="B136" s="5"/>
       <c r="C136" s="5"/>
       <c r="D136" s="5"/>
     </row>
-    <row r="137" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A137" s="4"/>
       <c r="B137" s="5"/>
       <c r="C137" s="5"/>
       <c r="D137" s="5"/>
     </row>
-    <row r="138" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A138" s="4"/>
       <c r="B138" s="5"/>
       <c r="C138" s="5"/>
       <c r="D138" s="5"/>
     </row>
-    <row r="139" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A139" s="4"/>
       <c r="B139" s="5"/>
       <c r="C139" s="5"/>
       <c r="D139" s="5"/>
     </row>
-    <row r="140" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A140" s="4"/>
       <c r="B140" s="5"/>
       <c r="C140" s="5"/>
       <c r="D140" s="5"/>
     </row>
-    <row r="141" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A141" s="4"/>
       <c r="B141" s="5"/>
       <c r="C141" s="5"/>
       <c r="D141" s="5"/>
     </row>
-    <row r="142" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A142" s="4"/>
       <c r="B142" s="5"/>
       <c r="C142" s="5"/>
       <c r="D142" s="5"/>
     </row>
-    <row r="143" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A143" s="4"/>
       <c r="B143" s="5"/>
       <c r="C143" s="5"/>
       <c r="D143" s="5"/>
     </row>
-    <row r="144" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A144" s="4"/>
       <c r="B144" s="5"/>
       <c r="C144" s="5"/>
       <c r="D144" s="5"/>
     </row>
-    <row r="145" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A145" s="4"/>
       <c r="B145" s="5"/>
       <c r="C145" s="5"/>
       <c r="D145" s="5"/>
     </row>
-    <row r="146" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A146" s="4"/>
       <c r="B146" s="5"/>
       <c r="C146" s="5"/>
       <c r="D146" s="5"/>
     </row>
-    <row r="147" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A147" s="4"/>
       <c r="B147" s="5"/>
       <c r="C147" s="5"/>
       <c r="D147" s="5"/>
     </row>
   </sheetData>
-  <sortState ref="A2:D26">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D26">
     <sortCondition ref="A1"/>
   </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
@@ -2548,91 +2550,91 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>

</xml_diff>